<commit_message>
Final preference matrix with preferences Jimmy
</commit_message>
<xml_diff>
--- a/Preference profiles/Preference matrix.xlsx
+++ b/Preference profiles/Preference matrix.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
   <si>
     <t>Chips</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Jimmy</t>
+  </si>
+  <si>
+    <t>Peronal-factor</t>
+  </si>
+  <si>
+    <t>DJ</t>
   </si>
 </sst>
 </file>
@@ -218,13 +224,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="41">
@@ -599,30 +608,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="36" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="13.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="C3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -632,8 +646,11 @@
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -646,8 +663,11 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -658,8 +678,11 @@
       <c r="D6" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -670,8 +693,11 @@
       <c r="D7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -682,161 +708,368 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" s="1">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="2"/>
       <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>36</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" s="1">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3</v>
+      </c>
+      <c r="E28" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="2"/>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" s="1">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="2"/>
       <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" s="1">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="2"/>
       <c r="B31" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -844,6 +1077,12 @@
       <c r="B33" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C33" s="1">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="105">
       <c r="A34" s="1" t="s">
@@ -855,6 +1094,9 @@
       <c r="D34" s="1">
         <v>1</v>
       </c>
+      <c r="E34" s="1">
+        <v>2</v>
+      </c>
       <c r="F34" s="1" t="s">
         <v>33</v>
       </c>
@@ -867,16 +1109,20 @@
         <v>0</v>
       </c>
       <c r="C35" s="1">
-        <f>ABS($C$34-C5)</f>
+        <f t="shared" ref="C35:C57" si="0">ABS($C$34-C5)</f>
         <v>2</v>
       </c>
       <c r="D35" s="1">
-        <f>ABS($D$34-D5)</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="1">
-        <f>SUM(C35:D35)</f>
-        <v>2</v>
+        <f t="shared" ref="D35:E57" si="1">ABS($D$34-D5)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <f>ABS($E$34-E5)</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="3">
+        <f>1/SUM(C35:E35)</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -885,16 +1131,20 @@
         <v>1</v>
       </c>
       <c r="C36" s="1">
-        <f>ABS($C$34-C6)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D36" s="1">
-        <f>ABS($D$34-D6)</f>
-        <v>2</v>
-      </c>
-      <c r="F36" s="1">
-        <f>SUM(C36:D36)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" ref="E36:E57" si="2">ABS($E$34-E6)</f>
+        <v>1</v>
+      </c>
+      <c r="F36" s="3">
+        <f t="shared" ref="F36:F57" si="3">1/SUM(C36:E36)</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -903,16 +1153,20 @@
         <v>2</v>
       </c>
       <c r="C37" s="1">
-        <f>ABS($C$34-C7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D37" s="1">
-        <f>ABS($D$34-D7)</f>
-        <v>1</v>
-      </c>
-      <c r="F37" s="1">
-        <f>SUM(C37:D37)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F37" s="3">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -921,15 +1175,19 @@
         <v>3</v>
       </c>
       <c r="C38" s="1">
-        <f>ABS($C$34-C8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D38" s="1">
-        <f>ABS($D$34-D8)</f>
-        <v>0</v>
-      </c>
-      <c r="F38" s="1">
-        <f>SUM(C38:D38)</f>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -941,16 +1199,20 @@
         <v>15</v>
       </c>
       <c r="C39" s="1">
-        <f>ABS($C$34-C9)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D39" s="1">
-        <f>ABS($D$34-D9)</f>
-        <v>1</v>
-      </c>
-      <c r="F39" s="1">
-        <f>SUM(C39:D39)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -959,16 +1221,20 @@
         <v>13</v>
       </c>
       <c r="C40" s="1">
-        <f>ABS($C$34-C10)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D40" s="1">
-        <f>ABS($D$34-D10)</f>
-        <v>1</v>
-      </c>
-      <c r="F40" s="1">
-        <f>SUM(C40:D40)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F40" s="3">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -977,16 +1243,20 @@
         <v>14</v>
       </c>
       <c r="C41" s="1">
-        <f>ABS($C$34-C11)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D41" s="1">
-        <f>ABS($D$34-D11)</f>
-        <v>1</v>
-      </c>
-      <c r="F41" s="1">
-        <f>SUM(C41:D41)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -995,16 +1265,20 @@
         <v>3</v>
       </c>
       <c r="C42" s="1">
-        <f>ABS($C$34-C12)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D42" s="1">
-        <f>ABS($D$34-D12)</f>
-        <v>1</v>
-      </c>
-      <c r="F42" s="1">
-        <f>SUM(C42:D42)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="3">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1015,16 +1289,20 @@
         <v>23</v>
       </c>
       <c r="C43" s="1">
-        <f>ABS($C$34-C13)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D43" s="1">
-        <f>ABS($D$34-D13)</f>
-        <v>1</v>
-      </c>
-      <c r="F43" s="1">
-        <f>SUM(C43:D43)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1033,16 +1311,20 @@
         <v>16</v>
       </c>
       <c r="C44" s="1">
-        <f>ABS($C$34-C14)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D44" s="1">
-        <f>ABS($D$34-D14)</f>
-        <v>1</v>
-      </c>
-      <c r="F44" s="1">
-        <f>SUM(C44:D44)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F44" s="3">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1051,16 +1333,20 @@
         <v>17</v>
       </c>
       <c r="C45" s="1">
-        <f>ABS($C$34-C15)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D45" s="1">
-        <f>ABS($D$34-D15)</f>
-        <v>1</v>
-      </c>
-      <c r="F45" s="1">
-        <f>SUM(C45:D45)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F45" s="3">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1069,16 +1355,20 @@
         <v>18</v>
       </c>
       <c r="C46" s="1">
-        <f>ABS($C$34-C16)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D46" s="1">
-        <f>ABS($D$34-D16)</f>
-        <v>1</v>
-      </c>
-      <c r="F46" s="1">
-        <f>SUM(C46:D46)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F46" s="3">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1089,16 +1379,20 @@
         <v>22</v>
       </c>
       <c r="C47" s="1">
-        <f>ABS($C$34-C17)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D47" s="1">
-        <f>ABS($D$34-D17)</f>
-        <v>1</v>
-      </c>
-      <c r="F47" s="1">
-        <f>SUM(C47:D47)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F47" s="3">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1107,16 +1401,20 @@
         <v>19</v>
       </c>
       <c r="C48" s="1">
-        <f>ABS($C$34-C18)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D48" s="1">
-        <f>ABS($D$34-D18)</f>
-        <v>1</v>
-      </c>
-      <c r="F48" s="1">
-        <f>SUM(C48:D48)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1125,16 +1423,20 @@
         <v>20</v>
       </c>
       <c r="C49" s="1">
-        <f>ABS($C$34-C19)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D49" s="1">
-        <f>ABS($D$34-D19)</f>
-        <v>1</v>
-      </c>
-      <c r="F49" s="1">
-        <f>SUM(C49:D49)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F49" s="3">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1143,16 +1445,20 @@
         <v>21</v>
       </c>
       <c r="C50" s="1">
-        <f>ABS($C$34-C20)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D50" s="1">
-        <f>ABS($D$34-D20)</f>
-        <v>1</v>
-      </c>
-      <c r="F50" s="1">
-        <f>SUM(C50:D50)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="3">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1163,16 +1469,20 @@
         <v>24</v>
       </c>
       <c r="C51" s="1">
-        <f>ABS($C$34-C21)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D51" s="1">
-        <f>ABS($D$34-D21)</f>
-        <v>1</v>
-      </c>
-      <c r="F51" s="1">
-        <f>SUM(C51:D51)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="3">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1181,16 +1491,20 @@
         <v>25</v>
       </c>
       <c r="C52" s="1">
-        <f>ABS($C$34-C22)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D52" s="1">
-        <f>ABS($D$34-D22)</f>
-        <v>1</v>
-      </c>
-      <c r="F52" s="1">
-        <f>SUM(C52:D52)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1199,16 +1513,20 @@
         <v>10</v>
       </c>
       <c r="C53" s="1">
-        <f>ABS($C$34-C23)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D53" s="1">
-        <f>ABS($D$34-D23)</f>
-        <v>1</v>
-      </c>
-      <c r="F53" s="1">
-        <f>SUM(C53:D53)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F53" s="3">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1219,16 +1537,20 @@
         <v>29</v>
       </c>
       <c r="C54" s="1">
-        <f>ABS($C$34-C24)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D54" s="1">
-        <f>ABS($D$34-D24)</f>
-        <v>1</v>
-      </c>
-      <c r="F54" s="1">
-        <f>SUM(C54:D54)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F54" s="3">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1237,16 +1559,20 @@
         <v>26</v>
       </c>
       <c r="C55" s="1">
-        <f>ABS($C$34-C25)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D55" s="1">
-        <f>ABS($D$34-D25)</f>
-        <v>1</v>
-      </c>
-      <c r="F55" s="1">
-        <f>SUM(C55:D55)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F55" s="3">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1255,16 +1581,20 @@
         <v>27</v>
       </c>
       <c r="C56" s="1">
-        <f>ABS($C$34-C26)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D56" s="1">
-        <f>ABS($D$34-D26)</f>
-        <v>1</v>
-      </c>
-      <c r="F56" s="1">
-        <f>SUM(C56:D56)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F56" s="3">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1273,16 +1603,20 @@
         <v>28</v>
       </c>
       <c r="C57" s="1">
-        <f>ABS($C$34-C27)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D57" s="1">
-        <f>ABS($D$34-D27)</f>
-        <v>1</v>
-      </c>
-      <c r="F57" s="1">
-        <f>SUM(C57:D57)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F57" s="3">
+        <f t="shared" si="3"/>
+        <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1293,18 +1627,20 @@
         <v>6</v>
       </c>
       <c r="C58" s="1">
+        <f>C28</f>
         <v>3</v>
       </c>
       <c r="D58" s="1">
+        <f>D28</f>
         <v>3</v>
       </c>
       <c r="E58" s="1">
-        <f>SUM(C58:D58)</f>
+        <f t="shared" ref="E58:E63" si="4">SUM(C58:D58)</f>
         <v>6</v>
       </c>
-      <c r="F58" s="1">
-        <f>E58/SUM($E$58:$E$63)</f>
-        <v>0.2608695652173913</v>
+      <c r="F58" s="3">
+        <f t="shared" ref="F58:F63" si="5">E58/SUM($E$58:$E$63)</f>
+        <v>0.27272727272727271</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1313,18 +1649,20 @@
         <v>7</v>
       </c>
       <c r="C59" s="1">
+        <f t="shared" ref="C59:D63" si="6">C29</f>
         <v>2</v>
       </c>
       <c r="D59" s="1">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E59" s="1">
-        <f>SUM(C59:D59)</f>
-        <v>3</v>
-      </c>
-      <c r="F59" s="1">
-        <f>E59/SUM($E$58:$E$63)</f>
-        <v>0.13043478260869565</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F59" s="3">
+        <f t="shared" si="5"/>
+        <v>0.13636363636363635</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1333,18 +1671,20 @@
         <v>8</v>
       </c>
       <c r="C60" s="1">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="D60" s="1">
-        <v>2</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="E60" s="1">
-        <f>SUM(C60:D60)</f>
-        <v>4</v>
-      </c>
-      <c r="F60" s="1">
-        <f>E60/SUM($E$58:$E$63)</f>
-        <v>0.17391304347826086</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F60" s="3">
+        <f t="shared" si="5"/>
+        <v>0.13636363636363635</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1353,18 +1693,20 @@
         <v>9</v>
       </c>
       <c r="C61" s="1">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="D61" s="1">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E61" s="1">
-        <f>SUM(C61:D61)</f>
-        <v>2</v>
-      </c>
-      <c r="F61" s="1">
-        <f>E61/SUM($E$58:$E$63)</f>
-        <v>8.6956521739130432E-2</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F61" s="3">
+        <f t="shared" si="5"/>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1373,18 +1715,20 @@
         <v>10</v>
       </c>
       <c r="C62" s="1">
-        <v>2</v>
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="D62" s="1">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="E62" s="1">
-        <f>SUM(C62:D62)</f>
-        <v>4</v>
-      </c>
-      <c r="F62" s="1">
-        <f>E62/SUM($E$58:$E$63)</f>
-        <v>0.17391304347826086</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="F62" s="3">
+        <f t="shared" si="5"/>
+        <v>0.22727272727272727</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1393,18 +1737,20 @@
         <v>11</v>
       </c>
       <c r="C63" s="1">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="D63" s="1">
-        <v>2</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="E63" s="1">
-        <f>SUM(C63:D63)</f>
-        <v>4</v>
-      </c>
-      <c r="F63" s="1">
-        <f>E63/SUM($E$58:$E$63)</f>
-        <v>0.17391304347826086</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F63" s="3">
+        <f t="shared" si="5"/>
+        <v>0.13636363636363635</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1415,22 +1761,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A51:A53"/>
     <mergeCell ref="A54:A57"/>
     <mergeCell ref="A28:A33"/>
-    <mergeCell ref="C3:D3"/>
     <mergeCell ref="A58:A63"/>
-    <mergeCell ref="C2:D2"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A24:A27"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A53"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>